<commit_message>
Made app being able to select the excel file to use, dropdown list of sheets and insert_row button working correctly per sheet intended, displays the newly-added row, some other minute mods.
</commit_message>
<xml_diff>
--- a/xxxxxmto_transmittal.xlsx
+++ b/xxxxxmto_transmittal.xlsx
@@ -472,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B:B D:D"/>
@@ -817,21 +817,53 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+      <c r="A15" s="7" t="inlineStr"/>
+      <c r="B15" s="7" t="inlineStr"/>
+      <c r="C15" s="7" t="inlineStr"/>
+      <c r="D15" s="7" t="inlineStr">
         <is>
           <t>125321565</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="7" t="inlineStr">
         <is>
           <t>21312</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>

</xml_diff>

<commit_message>
corrected data entry widget column-matching with the excel file. removed widget labels as the app will auto-read and set the labels to that of the headings of the sheets selected. other minute changes
</commit_message>
<xml_diff>
--- a/xxxxxmto_transmittal.xlsx
+++ b/xxxxxmto_transmittal.xlsx
@@ -2,43 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="test sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="dontSelectThis" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -59,56 +46,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -120,6 +76,7 @@
       </font>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -178,6 +135,14 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -468,416 +433,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B:B D:D"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col width="11.53" customWidth="1" style="6" min="3" max="3"/>
-    <col width="18.35" customWidth="1" style="7" min="6" max="6"/>
+    <col width="11.5703125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="18.28515625" customWidth="1" style="5" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Control #</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>DV</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Check Date</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Check #</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Payee</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="8">
-      <c r="A2" s="9" t="n">
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="2" t="n">
         <v>1111</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="3" t="n">
         <v>44931</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="2" t="n">
         <v>938555</v>
       </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>teppy</t>
         </is>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="4" t="n">
         <v>15000</v>
       </c>
-      <c r="G2" s="9" t="n"/>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" s="8">
-      <c r="A3" s="9" t="n">
+      <c r="G2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="2" t="n">
         <v>1112</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="3" t="n">
         <v>44932</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="2" t="n">
         <v>938556</v>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="G3" s="9" t="n"/>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="8">
-      <c r="A4" s="9" t="n">
+      <c r="G3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="2" t="n">
         <v>1113</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="3" t="n">
         <v>44934</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="2" t="n">
         <v>938557</v>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>imnasdjk</t>
         </is>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="4" t="n">
         <v>1114524</v>
       </c>
-      <c r="G4" s="9" t="n"/>
-    </row>
-    <row r="5" ht="12.75" customHeight="1" s="8">
-      <c r="A5" s="9" t="n">
+      <c r="G4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="2" t="n">
         <v>1114</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="3" t="n">
         <v>44940</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="2" t="n">
         <v>938558</v>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>pogi</t>
         </is>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="G5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="12.75" customHeight="1" s="8">
-      <c r="A6" s="9" t="n">
+      <c r="G5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="2" t="n">
         <v>1115</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="3" t="n">
         <v>44940</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="2" t="n">
         <v>938559</v>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>panget</t>
         </is>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="4" t="n">
         <v>1800</v>
       </c>
-      <c r="G6" s="9" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>Cancelled</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1" s="8">
-      <c r="A7" s="9" t="n">
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="2" t="n">
         <v>1116</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="3" t="n">
         <v>44948</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="2" t="n">
         <v>938560</v>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>ewan</t>
         </is>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="4" t="n">
         <v>2600</v>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>Stale</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1" s="8">
-      <c r="A8" s="9" t="n">
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="2" t="n">
         <v>1117</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="3" t="n">
         <v>44951</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="2" t="n">
         <v>938561</v>
       </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>kichan</t>
         </is>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" s="4" t="n">
         <v>25000</v>
       </c>
-      <c r="G8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="8">
-      <c r="A9" s="9" t="n">
+      <c r="G8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="2" t="n">
         <v>1118</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="3" t="n">
         <v>44954</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="2" t="n">
         <v>938562</v>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>loid</t>
         </is>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="4" t="n">
         <v>25000</v>
       </c>
-      <c r="G9" s="9" t="n"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1" s="8">
-      <c r="A10" s="9" t="n">
+      <c r="G9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="2" t="n">
         <v>1119</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="3" t="n">
         <v>44957</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="2" t="n">
         <v>938563</v>
       </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>phat</t>
         </is>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="4" t="n">
         <v>25000</v>
       </c>
-      <c r="G10" s="9" t="n"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>1120</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>01/31/23</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>938564</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>teppy</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="4" t="inlineStr">
         <is>
           <t>215000</t>
         </is>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="inlineStr"/>
-      <c r="B12" s="7" t="inlineStr"/>
-      <c r="C12" s="7" t="inlineStr"/>
-      <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="7" t="inlineStr"/>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>321321321</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
-        <is>
-          <t>1231</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr"/>
-      <c r="C13" s="7" t="inlineStr"/>
-      <c r="D13" s="7" t="inlineStr"/>
-      <c r="E13" s="7" t="inlineStr"/>
-      <c r="F13" s="7" t="inlineStr"/>
-      <c r="G13" s="7" t="inlineStr">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>payee</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="inlineStr"/>
-      <c r="B14" s="7" t="inlineStr"/>
-      <c r="C14" s="7" t="inlineStr"/>
-      <c r="D14" s="7" t="inlineStr"/>
-      <c r="E14" s="7" t="inlineStr"/>
-      <c r="F14" s="7" t="inlineStr"/>
-      <c r="G14" s="7" t="inlineStr">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>cd</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>cn</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>payee</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr"/>
-      <c r="B15" s="7" t="inlineStr"/>
-      <c r="C15" s="7" t="inlineStr"/>
-      <c r="D15" s="7" t="inlineStr">
-        <is>
-          <t>125321565</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="inlineStr"/>
-      <c r="F15" s="7" t="inlineStr">
-        <is>
-          <t>21312</t>
-        </is>
-      </c>
-      <c r="G15" s="7" t="inlineStr">
-        <is>
-          <t>Paid</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>sadf</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>asdfasdf</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Paid</t>
-        </is>
-      </c>
-    </row>
-    <row r="1048576" ht="12.75" customHeight="1" s="8"/>
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>one</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>more</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048569" ht="12.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576 D1:D1048576">
-    <cfRule type="duplicateValues" rank="0" priority="2" equalAverage="0" aboveAverage="0" dxfId="0" text="" percent="0" bottom="0"/>
+    <cfRule type="duplicateValues" priority="2" dxfId="0"/>
   </conditionalFormatting>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
@@ -886,4 +875,269 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>8/2/24</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>111222</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>teppy</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Stale</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>asf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>qas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>qs</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>qs</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ssa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AFAS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ASDFA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ASDF</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>select file widget</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>options to disable selection of certain sheets (for safety purposes ng dropdown lists)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>dropdown options page. (sama sama dapat lahat ng need na options per category sa isang column. Mods sa excel file ay auto-reflected sa options sa app)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>data validation per entry widget (merong options where blank=True pero almost every field, dapat required)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>nested enabled/disabled widgets based on prior selections</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>